<commit_message>
add idea 2 seminario
</commit_message>
<xml_diff>
--- a/SEMINARIO/Apuntes/Ideas/Ideas Germán Küber.xlsx
+++ b/SEMINARIO/Apuntes/Ideas/Ideas Germán Küber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5dfb7ada2583ab6/UAI/4º Año/SAP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Downloads\5TO\SEMINARIO\Apuntes\Ideas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F1CEED1B-5D00-4614-B99E-2A555269677B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C39F18F6-6F9A-471D-A140-6ED7902E2E76}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58076D6-FA5B-4B11-95F8-2C443E87D8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caratula" sheetId="1" r:id="rId1"/>
@@ -574,18 +574,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,11 +805,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.125" customWidth="1"/>
     <col min="2" max="26" width="7.625" customWidth="1"/>
@@ -1978,11 +1978,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.625" customWidth="1"/>
     <col min="2" max="6" width="9.375" customWidth="1"/>
@@ -3430,49 +3430,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="9"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="35" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="35" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="9"/>
@@ -3573,7 +3573,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="14"/>
       <c r="D12" s="12"/>
@@ -3588,13 +3588,13 @@
     <row r="13" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="35" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="11"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="35" t="s">
         <v>18</v>
       </c>
       <c r="I13" s="9"/>
@@ -3722,14 +3722,14 @@
       <c r="K23" s="17"/>
     </row>
     <row r="24" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="35" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="8"/>
@@ -3824,28 +3824,28 @@
     <row r="32" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="34"/>
     </row>
     <row r="35" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="32"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="32"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="32"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="32"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="32"/>
+      <c r="J36" s="35"/>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3959,11 +3959,11 @@
     <row r="46" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="11"/>
       <c r="C46" s="14"/>
-      <c r="D46" s="32"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="9"/>
       <c r="F46" s="11"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="32"/>
+      <c r="H46" s="35"/>
       <c r="I46" s="9"/>
       <c r="J46" s="11"/>
       <c r="K46" s="14"/>
@@ -4089,12 +4089,12 @@
       <c r="K56" s="17"/>
     </row>
     <row r="57" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="32"/>
+      <c r="B57" s="35"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="32"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
@@ -4187,7 +4187,7 @@
     <row r="65" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="33"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
@@ -4200,15 +4200,15 @@
     </row>
     <row r="68" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="32"/>
+      <c r="B69" s="35"/>
       <c r="C69" s="9"/>
-      <c r="D69" s="32"/>
+      <c r="D69" s="35"/>
       <c r="E69" s="9"/>
-      <c r="F69" s="32"/>
+      <c r="F69" s="35"/>
       <c r="G69" s="9"/>
-      <c r="H69" s="32"/>
+      <c r="H69" s="35"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="32"/>
+      <c r="J69" s="35"/>
       <c r="K69" s="9"/>
     </row>
     <row r="70" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4322,11 +4322,11 @@
     <row r="79" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="11"/>
       <c r="C79" s="14"/>
-      <c r="D79" s="32"/>
+      <c r="D79" s="35"/>
       <c r="E79" s="9"/>
       <c r="F79" s="11"/>
       <c r="G79" s="14"/>
-      <c r="H79" s="32"/>
+      <c r="H79" s="35"/>
       <c r="I79" s="9"/>
       <c r="J79" s="11"/>
       <c r="K79" s="14"/>
@@ -4452,12 +4452,12 @@
       <c r="K89" s="17"/>
     </row>
     <row r="90" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="32"/>
+      <c r="B90" s="35"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
       <c r="F90" s="9"/>
-      <c r="G90" s="32"/>
+      <c r="G90" s="35"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -5452,24 +5452,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C23"/>
-    <mergeCell ref="D3:E12"/>
-    <mergeCell ref="F3:G23"/>
-    <mergeCell ref="H3:I12"/>
-    <mergeCell ref="J3:K23"/>
-    <mergeCell ref="H13:I23"/>
-    <mergeCell ref="D13:E23"/>
-    <mergeCell ref="H36:I45"/>
-    <mergeCell ref="H46:I56"/>
-    <mergeCell ref="B24:F31"/>
-    <mergeCell ref="B36:C56"/>
-    <mergeCell ref="D36:E45"/>
-    <mergeCell ref="F36:G56"/>
-    <mergeCell ref="G24:K31"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="J36:K56"/>
-    <mergeCell ref="D46:E56"/>
     <mergeCell ref="B90:F97"/>
     <mergeCell ref="B57:F64"/>
     <mergeCell ref="G57:K64"/>
@@ -5482,6 +5464,24 @@
     <mergeCell ref="D69:E78"/>
     <mergeCell ref="D79:E89"/>
     <mergeCell ref="B69:C89"/>
+    <mergeCell ref="H36:I45"/>
+    <mergeCell ref="H46:I56"/>
+    <mergeCell ref="B24:F31"/>
+    <mergeCell ref="B36:C56"/>
+    <mergeCell ref="D36:E45"/>
+    <mergeCell ref="F36:G56"/>
+    <mergeCell ref="G24:K31"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="J36:K56"/>
+    <mergeCell ref="D46:E56"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C23"/>
+    <mergeCell ref="D3:E12"/>
+    <mergeCell ref="F3:G23"/>
+    <mergeCell ref="H3:I12"/>
+    <mergeCell ref="J3:K23"/>
+    <mergeCell ref="H13:I23"/>
+    <mergeCell ref="D13:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>